<commit_message>
Refactor code structure and remove redundant sections for improved readability
</commit_message>
<xml_diff>
--- a/backend/app/商品.xlsx
+++ b/backend/app/商品.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11805"/>
+    <workbookView windowWidth="14400" windowHeight="11805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,112 +29,11 @@
 </file>
 
 <file path=xl/cellimages.xml><?xml version="1.0" encoding="utf-8"?>
-<etc:cellImages xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <etc:cellImage>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="ID_84B235523A9049DFAA25A6242FDE1129" descr="屏幕截图 2026-01-11 010047"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2320925" y="635"/>
-          <a:ext cx="1057275" cy="1085850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-  </etc:cellImage>
-  <etc:cellImage>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="ID_44FF685DE8D74415859235B306B16B51" descr="屏幕截图 2026-01-11 010023"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2398395" y="1457960"/>
-          <a:ext cx="1067435" cy="1073785"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-  </etc:cellImage>
-  <etc:cellImage>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="ID_3A47F29225CA4E63AA463CC949C5E805" descr="屏幕截图 2026-01-11 010041"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4525010" y="298450"/>
-          <a:ext cx="2012315" cy="2007235"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-  </etc:cellImage>
-  <etc:cellImage>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="ID_35E43E71FD084BEB9EB8F47A39CAB908" descr="屏幕截图 2026-01-11 010028"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5443855" y="502920"/>
-          <a:ext cx="1070610" cy="1083945"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-  </etc:cellImage>
-</etc:cellImages>
+<etc:cellImages xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData"/>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>商品名称</t>
   </si>
@@ -145,10 +44,7 @@
     <t>价格</t>
   </si>
   <si>
-    <t>图片</t>
-  </si>
-  <si>
-    <t>标签</t>
+    <t>图片名称</t>
   </si>
   <si>
     <t>小金鱼</t>
@@ -157,22 +53,34 @@
     <t>手持烟花</t>
   </si>
   <si>
+    <t>xiaojinyu.png</t>
+  </si>
+  <si>
     <t>加特林</t>
   </si>
   <si>
     <t>升空类</t>
   </si>
   <si>
+    <t>jiatelin.png</t>
+  </si>
+  <si>
     <t>炮仗</t>
   </si>
   <si>
     <t>纸炮</t>
   </si>
   <si>
+    <t>paozhang.png</t>
+  </si>
+  <si>
     <t>蝴蝶王</t>
   </si>
   <si>
     <t>地面烟花</t>
+  </si>
+  <si>
+    <t>hudie.png</t>
   </si>
 </sst>
 </file>
@@ -1112,13 +1020,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="11.25" customWidth="1"/>
     <col min="4" max="4" width="12.5"/>
@@ -1126,7 +1034,7 @@
     <col min="7" max="7" width="12.3416666666667"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:5">
+    <row r="1" ht="18.75" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,26 +1047,22 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="75" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
-      <c r="D2" t="str">
-        <f>_xlfn.DISPIMG("ID_84B235523A9049DFAA25A6242FDE1129",1)</f>
-        <v>=DISPIMG("ID_84B235523A9049DFAA25A6242FDE1129",1)</v>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" ht="75" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1168,39 +1072,36 @@
       <c r="C3">
         <v>32</v>
       </c>
-      <c r="D3" t="str">
-        <f>_xlfn.DISPIMG("ID_35E43E71FD084BEB9EB8F47A39CAB908",1)</f>
-        <v>=DISPIMG("ID_35E43E71FD084BEB9EB8F47A39CAB908",1)</v>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" ht="74.8" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
-      <c r="D4" t="str">
-        <f>_xlfn.DISPIMG("ID_3A47F29225CA4E63AA463CC949C5E805",1)</f>
-        <v>=DISPIMG("ID_3A47F29225CA4E63AA463CC949C5E805",1)</v>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" ht="75" spans="1:5">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>23</v>
       </c>
-      <c r="D5" t="str">
-        <f>_xlfn.DISPIMG("ID_44FF685DE8D74415859235B306B16B51",1)</f>
-        <v>=DISPIMG("ID_44FF685DE8D74415859235B306B16B51",1)</v>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>